<commit_message>
feat: recommendation,compute total training time and add benchmark mode
</commit_message>
<xml_diff>
--- a/backend/calculator_model.xlsx
+++ b/backend/calculator_model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17775" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="13160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>GPU Type</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Recomended  Pipeline parallel degree</t>
+  </si>
+  <si>
+    <t>Recomended  microbatch size</t>
   </si>
   <si>
     <t>Optimizer States</t>
@@ -891,15 +894,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1242,26 +1242,26 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
-    <col min="2" max="2" width="14.6333333333333" customWidth="1"/>
-    <col min="3" max="3" width="12.2666666666667" customWidth="1"/>
-    <col min="4" max="4" width="20.2666666666667" customWidth="1"/>
-    <col min="5" max="5" width="11.7333333333333" customWidth="1"/>
-    <col min="6" max="6" width="12.7916666666667"/>
+    <col min="2" max="2" width="14.6346153846154" customWidth="1"/>
+    <col min="3" max="3" width="12.2692307692308" customWidth="1"/>
+    <col min="4" max="4" width="20.2692307692308" customWidth="1"/>
+    <col min="5" max="5" width="11.7307692307692" customWidth="1"/>
+    <col min="6" max="6" width="12.7884615384615"/>
     <col min="7" max="7" width="12.625"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.7916666666667"/>
-    <col min="10" max="10" width="14.2083333333333" customWidth="1"/>
-    <col min="11" max="11" width="12.7916666666667"/>
-    <col min="12" max="12" width="14.7333333333333" customWidth="1"/>
+    <col min="9" max="9" width="12.7884615384615"/>
+    <col min="10" max="10" width="14.2115384615385" customWidth="1"/>
+    <col min="11" max="11" width="12.7884615384615"/>
+    <col min="12" max="12" width="14.7307692307692" customWidth="1"/>
     <col min="13" max="13" width="11.375" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="11.2583333333333" customWidth="1"/>
-    <col min="16" max="16" width="15.2583333333333" customWidth="1"/>
+    <col min="15" max="15" width="11.2596153846154" customWidth="1"/>
+    <col min="16" max="16" width="15.2596153846154" customWidth="1"/>
     <col min="17" max="17" width="11.375" customWidth="1"/>
     <col min="18" max="18" width="11.125" customWidth="1"/>
     <col min="19" max="19" width="10.625" customWidth="1"/>
@@ -1269,10 +1269,10 @@
     <col min="21" max="21" width="9.375"/>
     <col min="22" max="22" width="10.625" customWidth="1"/>
     <col min="23" max="23" width="9.875" customWidth="1"/>
-    <col min="26" max="26" width="10.7583333333333" customWidth="1"/>
+    <col min="26" max="26" width="10.7596153846154" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="57" spans="1:8">
+    <row r="1" ht="69" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1282,113 +1282,113 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:8">
-      <c r="A2" s="9">
+    <row r="2" spans="1:8">
+      <c r="A2" s="8">
         <v>3090</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>142</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>36</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>24</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>936</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>64</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="9">
         <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>1499</v>
       </c>
     </row>
-    <row r="5" ht="42.75" spans="1:6">
-      <c r="A5" s="9" t="s">
+    <row r="5" ht="51" spans="1:6">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" ht="28.5" spans="1:6">
-      <c r="A6" s="9" t="s">
+    <row r="6" ht="34" spans="1:6">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>2048</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>16</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>1024</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>96</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>50257</v>
       </c>
     </row>
-    <row r="9" ht="28.5" spans="1:2">
+    <row r="9" ht="35" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="42.75" spans="1:8">
+    <row r="12" ht="52" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>100</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1410,236 +1410,243 @@
   <sheetPr/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <sheetData>
-    <row r="1" ht="42.75" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="52" spans="1:10">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="e">
+      <c r="B1" s="4" t="e">
         <f>$E1+#REF!*($G1+$I1)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="e">
+      <c r="D1" s="4" t="e">
         <f>#REF!*#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="e">
+      <c r="F1" s="4" t="e">
         <f>4*#REF!*#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="5" t="e">
+      <c r="H1" s="4" t="e">
         <f>8*#REF!*#REF!++#REF!*5</f>
         <v>#REF!</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="8" t="e">
+      <c r="J1" s="7" t="e">
         <f>#REF!*#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" ht="71.25" spans="1:4">
+    <row r="4" ht="86" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="7" t="e">
+      <c r="B4" s="6" t="e">
         <f>MAX(FLOOR(3*#REF!/#REF!*#REF!/2/1000,1),1)</f>
         <v>#REF!</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="7" t="e">
+      <c r="D4" s="6" t="e">
         <f>CEILING((#REF!*C1*#REF!*2/B4+16*#REF!/B4)/#REF!/1000000000,1)</f>
         <v>#REF!</v>
       </c>
-    </row>
-    <row r="7" ht="28.5" spans="1:10">
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="6" t="e">
+        <f>CEILING((#REF!*E1*#REF!*2/D4+16*#REF!/D4)/#REF!/1000000000,1)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="7" ht="52" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="e">
         <f>12*#REF!/B4/D4</f>
         <v>#REF!</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="e">
         <f>2*#REF!/B4/D4</f>
         <v>#REF!</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="e">
         <f>2*#REF!/B4/D4</f>
         <v>#REF!</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2" t="e">
         <f>#REF!*#REF!*#REF!*2/B4</f>
         <v>#REF!</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2" t="e">
         <f>(B7+D7+F7+H7)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" ht="57" spans="1:12">
+    <row r="10" ht="121" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="e">
         <f>#REF!/D4</f>
         <v>#REF!</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2" t="e">
         <f>#REF!/H4</f>
         <v>#REF!</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="2" t="e">
         <f>2*#REF!*#REF!*#REF!/B4/D4/#REF!/1000000000000</f>
         <v>#REF!</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10" s="2" t="e">
         <f>6*#REF!*#REF!*#REF!/B4/D4/#REF!/1000000000000</f>
         <v>#REF!</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J10" s="2" t="e">
         <f>F10/B10/D10</f>
         <v>#REF!</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L10" s="2" t="e">
         <f>H10/B10/D10</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" ht="57" spans="1:4">
+    <row r="13" ht="69" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="2" t="e">
         <f>#REF!/E4</f>
         <v>#REF!</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="e">
         <f>#REF!/I4</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" ht="57" spans="1:4">
+    <row r="14" ht="86" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="e">
         <f>2*#REF!*#REF!*#REF!*#REF!/E4/#REF!/1000000000*2</f>
         <v>#REF!</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="e">
         <f>B14/B13/D13</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="15" ht="57" spans="1:4">
+    <row r="15" ht="104" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="e">
         <f>2*#REF!*#REF!*#REF!*#REF!/E4/#REF!/1000000000*2</f>
         <v>#REF!</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2" t="e">
         <f>B15/B13/D13</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="16" ht="71.25" spans="1:4">
+    <row r="16" ht="121" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="2" t="e">
         <f>B15/C4*2</f>
         <v>#REF!</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2" t="e">
         <f>B16/B13/D13</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="17" ht="28.5" spans="1:4">
+    <row r="17" ht="69" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2" t="e">
         <f>2*#REF!*#REF!*#REF!/C4/G4*8/1000000000*8</f>
         <v>#REF!</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="e">
         <f>B17/D13</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="18" ht="71.25" spans="1:4">
+    <row r="18" ht="86" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="e">
         <f>2*#REF!*2*8/1000000000/C4/G4</f>
         <v>#REF!</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="e">
         <f>#REF!/C4/E4*2*8*2/1000000000*8/G4</f>
@@ -1658,175 +1665,175 @@
   <sheetPr/>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4"/>
   <cols>
     <col min="8" max="8" width="12.625"/>
     <col min="10" max="10" width="12.625"/>
     <col min="14" max="14" width="12.625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="57" spans="1:16">
+    <row r="1" ht="69" spans="1:16">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2">
         <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="e">
         <f>(#REF!-1)*H1/#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H1" s="2" t="e">
         <f>#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="2" t="e">
         <f>MAX(#REF!+#REF!,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L1" s="2" t="e">
         <f>(#REF!-1)*J1/#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N1" s="2">
         <v>0.4031725568</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P1" s="2" t="e">
         <f>F1+H1+J1+L1</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="2" ht="57" spans="1:16">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+    <row r="2" ht="104" spans="1:16">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="3">
+        <v>40</v>
+      </c>
+      <c r="H2" s="2">
         <v>0.000131072</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="3">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2">
         <v>0.000131072</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" ht="71.25" spans="1:16">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" ht="121" spans="1:16">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="3" t="e">
+        <v>54</v>
+      </c>
+      <c r="H3" s="2" t="e">
         <f>#REF!/#REF!/#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="3">
+        <v>44</v>
+      </c>
+      <c r="J3" s="2">
         <v>0.000131072</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" ht="57" spans="1:16">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" ht="121" spans="1:16">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="3" t="e">
+        <v>55</v>
+      </c>
+      <c r="H4" s="2" t="e">
         <f>H3/(H2+H3)</f>
         <v>#REF!</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="3">
+        <v>56</v>
+      </c>
+      <c r="J4" s="2">
         <f>0.290738519833239/B1/D1</f>
         <v>0.000757131562065727</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" ht="28.5" spans="1:16">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" ht="35" spans="1:16">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="3">
+        <v>55</v>
+      </c>
+      <c r="J5" s="2">
         <f>J4/J4</f>
         <v>1</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>